<commit_message>
Fixed BM2 section labels in the metadata
</commit_message>
<xml_diff>
--- a/data/V10F24_041_spots_seurat_metadata.xlsx
+++ b/data/V10F24_041_spots_seurat_metadata.xlsx
@@ -896,139 +896,427 @@
     <t xml:space="preserve">V10F24_041_B1</t>
   </si>
   <si>
+    <t xml:space="preserve">BM2_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V10F24_041_B1_BM2_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GGAGGATTGAAAGGAG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BM2_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V10F24_041_B1_BM2_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCGCTGGTGCCATTCA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTTAGAGTGTGCCGCT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCGGAATGACCATCAA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GATGTGTTGTCACAAG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCGCATTCAATGACTT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTGGTTCAACGCATCA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTCAGTTGTGCTCGTT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTGACGTAACTCGGT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GATGTCGGTCAACTGC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCAACACATTGGGTAA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTGTATACGCGAGCA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTGAAACGTGCTCCAC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAGATCCGAAGTCGCA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGAAACTTATGCAAGC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CGTTGAGTAATTGCGT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BM2_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V10F24_041_B1_BM2_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAAATGCCGTCTCATG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GGTCGGTAATTAGACA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGCGGGAAGGGTCCAT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTAGACGTCGTTACAT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCTAGTTAGTCGCATG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GAAACTCTAATGAAGG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTGTATCACACAGAAT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCGACGTAAACACAAC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTCCATCATGCGGTGA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGCACAGTGAAGTTAT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGCGAGCCCTTCCGCG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AACCCAGAGACGGAGA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GAAGAACGGTGCAGGT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTGCGTGAACGCTTAG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCGCCTGCGAATTGGT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGATGAGGGTTGCGAT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTACTTGGGCACTTCT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCTCACCAATCTTGAC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCTAGTTTCATTGAGG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGGACATCGCACGTCG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTTGGATTCAGTGGCT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAAAGCTGCAATAGGG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGAAGAGCGGTCCTAG-1_2</t>
+  </si>
+  <si>
     <t xml:space="preserve">BM2_4</t>
   </si>
   <si>
     <t xml:space="preserve">V10F24_041_B1_BM2_4</t>
   </si>
   <si>
-    <t xml:space="preserve">GGAGGATTGAAAGGAG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BM2_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V10F24_041_B1_BM2_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCGCTGGTGCCATTCA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTTAGAGTGTGCCGCT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCGGAATGACCATCAA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GATGTGTTGTCACAAG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCGCATTCAATGACTT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTGGTTCAACGCATCA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTCAGTTGTGCTCGTT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATTGACGTAACTCGGT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GATGTCGGTCAACTGC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCAACACATTGGGTAA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTGTATACGCGAGCA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTGAAACGTGCTCCAC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAGATCCGAAGTCGCA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TGAAACTTATGCAAGC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CGTTGAGTAATTGCGT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BM2_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V10F24_041_B1_BM2_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAAATGCCGTCTCATG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GGTCGGTAATTAGACA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGCGGGAAGGGTCCAT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTAGACGTCGTTACAT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCTAGTTAGTCGCATG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GAAACTCTAATGAAGG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTGTATCACACAGAAT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCGACGTAAACACAAC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTCCATCATGCGGTGA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TGCACAGTGAAGTTAT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TGCGAGCCCTTCCGCG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AACCCAGAGACGGAGA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GAAGAACGGTGCAGGT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTGCGTGAACGCTTAG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCGCCTGCGAATTGGT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGATGAGGGTTGCGAT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTACTTGGGCACTTCT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCTCACCAATCTTGAC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GCTAGTTTCATTGAGG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGGACATCGCACGTCG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTTGGATTCAGTGGCT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAAAGCTGCAATAGGG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TGAAGAGCGGTCCTAG-1_2</t>
+    <t xml:space="preserve">ACGTTATTGGTCACTC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTCTTAGTGAACGGTG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGGACGCTCGATGTTG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GGGATACGGTAATAAT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGTTCACCGGTTGGAC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGACACCGTTGCTTG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTCTGTTTCCTGTCGC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TACATGACCTTATCCG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTCCTTCTACAACCCA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TATATGCTGGGTTGCC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTCTCGCTGTACTATG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AATAGTCGCGAGTCGG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGTTACCCTTAAGACT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTAAATAAGACCCAT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTGAGTCTAAGACGGA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GGACTAAGTCAGGAGT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTCAGTTTGTGGCAGC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTAGCCCGGATAGTG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GATGCGAATGGTATTA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCTAACTGTATGTAAA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GAGAGCGCAGTCCCTG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CATCTGCAGGATCATT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAGTGCAAAGGTAGAC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATCTGCACCTCTGCGA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BM2_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V10F24_041_B1_BM2_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCTCACCTGAGGGAGC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGTGAGCCTCGCCGCC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCATACCTTTACTTGT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTAATAAAGGGCTCCC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTGAACTCCCATTCGA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTGGTTACTTCTTTCG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTTACTAAGTCCATT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GGGTGCATATGAAAGC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGATGGCTGTTTCTGA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCACTATCCGGGTCAC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CGCGGTAAGTCTAGCT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCGGGCATTACGATGC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTCGGGATAACACCTA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTCCCGAATTCGTTT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTTCATCGTTTGGCTG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTTTACCCTCATGAA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCGAGAGTTGCGTCCA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTTCGGGCGTACCATT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CGACTTTGTATAGCCT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCCATCGATGCTGCAT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAACACATCTCCTGCC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GGCAGAGAGATCGGGA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BM2_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V10F24_041_B1_BM2_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTCCTCTGCCCGAATA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCCGCATTAGTCCGGC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTACGCACGGAGTACC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BM2_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V10F24_041_B1_BM2_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAATTAACGGGTAGCT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CGGCCACGCACAAAGT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAGGTTCGAGTTCGTC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GAATTATAGTGAAAGG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCGCTAATTGAATAGA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GGTAGTGCTCGCACCA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TATTCAATTCTAATCC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTCAAAGTCTCTAGCC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAGAGCTCTTTATCGG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTAACGTTAAAGCCTG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAGCGCCAACACGATA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTGCTGCAGATAAGGA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTCGTACCTACGATTG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGAATAAATCTTCAGG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTCTACTCAATTACAA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGTAATGACCACAATA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGTGCTTTACGTAAGA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TATAGGGTACTCATGA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCAGCTGATGGTACTT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTCATTGTCAGTGGA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCTGTCGCCCGTAAAT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTACACTTACCTGAAG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATGGAGCAGGCCGTGA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAGACTGCAAGCTACT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCGCACAAAGACCAAC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCGATTGTTAACGTTA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTCGTCAGTAATCCC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AATCTCTACTGTGGTT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCACTGGTGGCTGGTT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GACAGGCACACACTAT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCAACGCGACCGGCAG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGCTCTAGACGTTCCA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTTCTATTAATGCTAG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BM2_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V10F24_041_B1_BM2_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATGGAAATTTAAGGAG-1_2</t>
   </si>
   <si>
     <t xml:space="preserve">BM2_5</t>
@@ -1037,277 +1325,40 @@
     <t xml:space="preserve">V10F24_041_B1_BM2_5</t>
   </si>
   <si>
-    <t xml:space="preserve">ACGTTATTGGTCACTC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTCTTAGTGAACGGTG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGGACGCTCGATGTTG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GGGATACGGTAATAAT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGTTCACCGGTTGGAC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TGGACACCGTTGCTTG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTCTGTTTCCTGTCGC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TACATGACCTTATCCG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTCCTTCTACAACCCA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TATATGCTGGGTTGCC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTCTCGCTGTACTATG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AATAGTCGCGAGTCGG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGTTACCCTTAAGACT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTAAATAAGACCCAT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTGAGTCTAAGACGGA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GGACTAAGTCAGGAGT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTCAGTTTGTGGCAGC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTAGCCCGGATAGTG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GATGCGAATGGTATTA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCTAACTGTATGTAAA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GAGAGCGCAGTCCCTG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CATCTGCAGGATCATT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AAGTGCAAAGGTAGAC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATCTGCACCTCTGCGA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BM2_10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V10F24_041_B1_BM2_10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCTCACCTGAGGGAGC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGTGAGCCTCGCCGCC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCATACCTTTACTTGT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTAATAAAGGGCTCCC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTGAACTCCCATTCGA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTGGTTACTTCTTTCG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATTTACTAAGTCCATT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GGGTGCATATGAAAGC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TGATGGCTGTTTCTGA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCACTATCCGGGTCAC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CGCGGTAAGTCTAGCT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GCGGGCATTACGATGC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTCGGGATAACACCTA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTCCCGAATTCGTTT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTTCATCGTTTGGCTG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTTTACCCTCATGAA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GCGAGAGTTGCGTCCA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTTCGGGCGTACCATT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CGACTTTGTATAGCCT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GCCATCGATGCTGCAT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAACACATCTCCTGCC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GGCAGAGAGATCGGGA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BM2_12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V10F24_041_B1_BM2_12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTCCTCTGCCCGAATA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GCCGCATTAGTCCGGC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTACGCACGGAGTACC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BM2_11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V10F24_041_B1_BM2_11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AAATTAACGGGTAGCT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CGGCCACGCACAAAGT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAGGTTCGAGTTCGTC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GAATTATAGTGAAAGG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GCGCTAATTGAATAGA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GGTAGTGCTCGCACCA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TATTCAATTCTAATCC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTCAAAGTCTCTAGCC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AAGAGCTCTTTATCGG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTAACGTTAAAGCCTG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAGCGCCAACACGATA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTGCTGCAGATAAGGA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTCGTACCTACGATTG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGAATAAATCTTCAGG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTCTACTCAATTACAA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TGTAATGACCACAATA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TGTGCTTTACGTAAGA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TATAGGGTACTCATGA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCAGCTGATGGTACTT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTCATTGTCAGTGGA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCTGTCGCCCGTAAAT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTACACTTACCTGAAG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATGGAGCAGGCCGTGA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AAGACTGCAAGCTACT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCGCACAAAGACCAAC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GCGATTGTTAACGTTA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTCGTCAGTAATCCC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AATCTCTACTGTGGTT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCACTGGTGGCTGGTT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GACAGGCACACACTAT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCAACGCGACCGGCAG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGCTCTAGACGTTCCA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTTCTATTAATGCTAG-1_2</t>
+    <t xml:space="preserve">ACTGCTCGGAAGGATG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAGCGATTCCCTTCAA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCTAGCTTGAATAGCT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTGCGGCATCAGAAAG-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AATAGAACAGAGTGGC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACACTGATCAAGGTGT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTCCTACTCTACGGGC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTCGAGACATACGATA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TATCAGTGGCGTAGTC-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGATACATTTAGCCGT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTCCGGCCTTGAGGCT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GGTGGACTGCTCTGGC-1_2</t>
   </si>
   <si>
     <t xml:space="preserve">BM2_7</t>
@@ -1316,73 +1367,22 @@
     <t xml:space="preserve">V10F24_041_B1_BM2_7</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGGAAATTTAAGGAG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BM2_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V10F24_041_B1_BM2_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTGCTCGGAAGGATG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAGCGATTCCCTTCAA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GCTAGCTTGAATAGCT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTGCGGCATCAGAAAG-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AATAGAACAGAGTGGC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACACTGATCAAGGTGT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTCCTACTCTACGGGC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTCGAGACATACGATA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TATCAGTGGCGTAGTC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TGATACATTTAGCCGT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTCCGGCCTTGAGGCT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GGTGGACTGCTCTGGC-1_2</t>
+    <t xml:space="preserve">TTGAGAAGTTTAGCAT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTCCGGACCTGAAATT-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTGTGGTCGGGAGATA-1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTATTATCTGGAAGGC-1_2</t>
   </si>
   <si>
     <t xml:space="preserve">BM2_8</t>
   </si>
   <si>
     <t xml:space="preserve">V10F24_041_B1_BM2_8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTGAGAAGTTTAGCAT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTCCGGACCTGAAATT-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTGTGGTCGGGAGATA-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTATTATCTGGAAGGC-1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BM2_9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V10F24_041_B1_BM2_9</t>
   </si>
   <si>
     <t xml:space="preserve">AAATCGCGGAAGGAGT-1_2</t>
@@ -15083,7 +15083,7 @@
         <v>222</v>
       </c>
       <c r="G242" t="s">
-        <v>222</v>
+        <v>22</v>
       </c>
       <c r="H242" t="s">
         <v>43</v>
@@ -15136,7 +15136,7 @@
         <v>22</v>
       </c>
       <c r="G243" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="H243" t="s">
         <v>43</v>
@@ -15189,7 +15189,7 @@
         <v>22</v>
       </c>
       <c r="G244" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="H244" t="s">
         <v>43</v>
@@ -15242,7 +15242,7 @@
         <v>22</v>
       </c>
       <c r="G245" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="H245" t="s">
         <v>43</v>
@@ -15295,7 +15295,7 @@
         <v>22</v>
       </c>
       <c r="G246" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="H246" t="s">
         <v>43</v>
@@ -15348,7 +15348,7 @@
         <v>22</v>
       </c>
       <c r="G247" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="H247" t="s">
         <v>43</v>
@@ -15401,7 +15401,7 @@
         <v>222</v>
       </c>
       <c r="G248" t="s">
-        <v>222</v>
+        <v>22</v>
       </c>
       <c r="H248" t="s">
         <v>43</v>
@@ -15454,7 +15454,7 @@
         <v>222</v>
       </c>
       <c r="G249" t="s">
-        <v>222</v>
+        <v>22</v>
       </c>
       <c r="H249" t="s">
         <v>43</v>
@@ -15507,7 +15507,7 @@
         <v>22</v>
       </c>
       <c r="G250" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="H250" t="s">
         <v>43</v>
@@ -15560,7 +15560,7 @@
         <v>22</v>
       </c>
       <c r="G251" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="H251" t="s">
         <v>43</v>
@@ -15613,7 +15613,7 @@
         <v>22</v>
       </c>
       <c r="G252" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="H252" t="s">
         <v>43</v>
@@ -15666,7 +15666,7 @@
         <v>222</v>
       </c>
       <c r="G253" t="s">
-        <v>222</v>
+        <v>22</v>
       </c>
       <c r="H253" t="s">
         <v>43</v>
@@ -15719,7 +15719,7 @@
         <v>222</v>
       </c>
       <c r="G254" t="s">
-        <v>222</v>
+        <v>22</v>
       </c>
       <c r="H254" t="s">
         <v>43</v>
@@ -15772,7 +15772,7 @@
         <v>222</v>
       </c>
       <c r="G255" t="s">
-        <v>222</v>
+        <v>22</v>
       </c>
       <c r="H255" t="s">
         <v>43</v>
@@ -15825,7 +15825,7 @@
         <v>22</v>
       </c>
       <c r="G256" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="H256" t="s">
         <v>43</v>
@@ -15878,7 +15878,7 @@
         <v>22</v>
       </c>
       <c r="G257" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="H257" t="s">
         <v>43</v>
@@ -15931,7 +15931,7 @@
         <v>43</v>
       </c>
       <c r="G258" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="H258" t="s">
         <v>43</v>
@@ -15984,7 +15984,7 @@
         <v>43</v>
       </c>
       <c r="G259" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="H259" t="s">
         <v>43</v>
@@ -16037,7 +16037,7 @@
         <v>222</v>
       </c>
       <c r="G260" t="s">
-        <v>222</v>
+        <v>22</v>
       </c>
       <c r="H260" t="s">
         <v>43</v>
@@ -16090,7 +16090,7 @@
         <v>222</v>
       </c>
       <c r="G261" t="s">
-        <v>222</v>
+        <v>22</v>
       </c>
       <c r="H261" t="s">
         <v>43</v>
@@ -16143,7 +16143,7 @@
         <v>222</v>
       </c>
       <c r="G262" t="s">
-        <v>222</v>
+        <v>22</v>
       </c>
       <c r="H262" t="s">
         <v>43</v>
@@ -16196,7 +16196,7 @@
         <v>22</v>
       </c>
       <c r="G263" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="H263" t="s">
         <v>43</v>
@@ -16249,7 +16249,7 @@
         <v>22</v>
       </c>
       <c r="G264" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="H264" t="s">
         <v>43</v>
@@ -16302,7 +16302,7 @@
         <v>22</v>
       </c>
       <c r="G265" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="H265" t="s">
         <v>43</v>
@@ -16355,7 +16355,7 @@
         <v>43</v>
       </c>
       <c r="G266" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="H266" t="s">
         <v>43</v>
@@ -16408,7 +16408,7 @@
         <v>43</v>
       </c>
       <c r="G267" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="H267" t="s">
         <v>43</v>
@@ -16461,7 +16461,7 @@
         <v>43</v>
       </c>
       <c r="G268" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="H268" t="s">
         <v>43</v>
@@ -16514,7 +16514,7 @@
         <v>43</v>
       </c>
       <c r="G269" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="H269" t="s">
         <v>43</v>
@@ -16567,7 +16567,7 @@
         <v>222</v>
       </c>
       <c r="G270" t="s">
-        <v>222</v>
+        <v>22</v>
       </c>
       <c r="H270" t="s">
         <v>43</v>
@@ -16620,7 +16620,7 @@
         <v>222</v>
       </c>
       <c r="G271" t="s">
-        <v>222</v>
+        <v>22</v>
       </c>
       <c r="H271" t="s">
         <v>43</v>
@@ -16673,7 +16673,7 @@
         <v>43</v>
       </c>
       <c r="G272" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="H272" t="s">
         <v>43</v>
@@ -16726,7 +16726,7 @@
         <v>43</v>
       </c>
       <c r="G273" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="H273" t="s">
         <v>43</v>
@@ -16779,7 +16779,7 @@
         <v>43</v>
       </c>
       <c r="G274" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="H274" t="s">
         <v>43</v>
@@ -16832,7 +16832,7 @@
         <v>222</v>
       </c>
       <c r="G275" t="s">
-        <v>222</v>
+        <v>22</v>
       </c>
       <c r="H275" t="s">
         <v>43</v>
@@ -16885,7 +16885,7 @@
         <v>222</v>
       </c>
       <c r="G276" t="s">
-        <v>222</v>
+        <v>22</v>
       </c>
       <c r="H276" t="s">
         <v>43</v>
@@ -16938,7 +16938,7 @@
         <v>222</v>
       </c>
       <c r="G277" t="s">
-        <v>222</v>
+        <v>22</v>
       </c>
       <c r="H277" t="s">
         <v>43</v>
@@ -16991,7 +16991,7 @@
         <v>222</v>
       </c>
       <c r="G278" t="s">
-        <v>222</v>
+        <v>22</v>
       </c>
       <c r="H278" t="s">
         <v>43</v>
@@ -17044,7 +17044,7 @@
         <v>43</v>
       </c>
       <c r="G279" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="H279" t="s">
         <v>43</v>
@@ -17097,7 +17097,7 @@
         <v>43</v>
       </c>
       <c r="G280" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="H280" t="s">
         <v>43</v>
@@ -17150,7 +17150,7 @@
         <v>216</v>
       </c>
       <c r="G281" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H281" t="s">
         <v>43</v>
@@ -17203,7 +17203,7 @@
         <v>216</v>
       </c>
       <c r="G282" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H282" t="s">
         <v>43</v>
@@ -17256,7 +17256,7 @@
         <v>222</v>
       </c>
       <c r="G283" t="s">
-        <v>222</v>
+        <v>22</v>
       </c>
       <c r="H283" t="s">
         <v>43</v>
@@ -17309,7 +17309,7 @@
         <v>43</v>
       </c>
       <c r="G284" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="H284" t="s">
         <v>43</v>
@@ -17362,7 +17362,7 @@
         <v>216</v>
       </c>
       <c r="G285" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H285" t="s">
         <v>43</v>
@@ -17415,7 +17415,7 @@
         <v>216</v>
       </c>
       <c r="G286" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H286" t="s">
         <v>43</v>
@@ -17468,7 +17468,7 @@
         <v>216</v>
       </c>
       <c r="G287" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H287" t="s">
         <v>43</v>
@@ -17521,7 +17521,7 @@
         <v>216</v>
       </c>
       <c r="G288" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H288" t="s">
         <v>43</v>
@@ -17574,7 +17574,7 @@
         <v>216</v>
       </c>
       <c r="G289" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H289" t="s">
         <v>43</v>
@@ -17627,7 +17627,7 @@
         <v>216</v>
       </c>
       <c r="G290" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H290" t="s">
         <v>43</v>
@@ -17680,7 +17680,7 @@
         <v>216</v>
       </c>
       <c r="G291" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H291" t="s">
         <v>43</v>
@@ -17733,7 +17733,7 @@
         <v>216</v>
       </c>
       <c r="G292" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H292" t="s">
         <v>43</v>
@@ -17786,7 +17786,7 @@
         <v>216</v>
       </c>
       <c r="G293" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H293" t="s">
         <v>43</v>
@@ -17839,7 +17839,7 @@
         <v>216</v>
       </c>
       <c r="G294" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H294" t="s">
         <v>43</v>
@@ -17892,7 +17892,7 @@
         <v>216</v>
       </c>
       <c r="G295" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H295" t="s">
         <v>43</v>
@@ -17945,7 +17945,7 @@
         <v>216</v>
       </c>
       <c r="G296" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H296" t="s">
         <v>43</v>
@@ -17998,7 +17998,7 @@
         <v>216</v>
       </c>
       <c r="G297" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H297" t="s">
         <v>43</v>
@@ -18051,7 +18051,7 @@
         <v>216</v>
       </c>
       <c r="G298" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H298" t="s">
         <v>43</v>
@@ -18104,7 +18104,7 @@
         <v>216</v>
       </c>
       <c r="G299" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H299" t="s">
         <v>43</v>
@@ -18157,7 +18157,7 @@
         <v>216</v>
       </c>
       <c r="G300" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H300" t="s">
         <v>43</v>
@@ -18210,7 +18210,7 @@
         <v>216</v>
       </c>
       <c r="G301" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H301" t="s">
         <v>43</v>
@@ -18263,7 +18263,7 @@
         <v>216</v>
       </c>
       <c r="G302" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H302" t="s">
         <v>43</v>
@@ -18316,7 +18316,7 @@
         <v>216</v>
       </c>
       <c r="G303" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H303" t="s">
         <v>43</v>
@@ -18369,7 +18369,7 @@
         <v>216</v>
       </c>
       <c r="G304" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H304" t="s">
         <v>43</v>
@@ -18422,7 +18422,7 @@
         <v>365</v>
       </c>
       <c r="G305" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H305" t="s">
         <v>43</v>
@@ -18475,7 +18475,7 @@
         <v>365</v>
       </c>
       <c r="G306" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H306" t="s">
         <v>43</v>
@@ -18528,7 +18528,7 @@
         <v>365</v>
       </c>
       <c r="G307" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H307" t="s">
         <v>43</v>
@@ -18581,7 +18581,7 @@
         <v>365</v>
       </c>
       <c r="G308" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H308" t="s">
         <v>43</v>
@@ -18634,7 +18634,7 @@
         <v>365</v>
       </c>
       <c r="G309" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H309" t="s">
         <v>43</v>
@@ -18687,7 +18687,7 @@
         <v>365</v>
       </c>
       <c r="G310" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H310" t="s">
         <v>43</v>
@@ -18740,7 +18740,7 @@
         <v>365</v>
       </c>
       <c r="G311" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H311" t="s">
         <v>43</v>
@@ -18793,7 +18793,7 @@
         <v>365</v>
       </c>
       <c r="G312" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H312" t="s">
         <v>43</v>
@@ -18846,7 +18846,7 @@
         <v>365</v>
       </c>
       <c r="G313" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H313" t="s">
         <v>43</v>
@@ -18899,7 +18899,7 @@
         <v>365</v>
       </c>
       <c r="G314" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H314" t="s">
         <v>43</v>
@@ -18952,7 +18952,7 @@
         <v>365</v>
       </c>
       <c r="G315" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H315" t="s">
         <v>43</v>
@@ -19005,7 +19005,7 @@
         <v>365</v>
       </c>
       <c r="G316" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H316" t="s">
         <v>43</v>
@@ -19058,7 +19058,7 @@
         <v>365</v>
       </c>
       <c r="G317" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H317" t="s">
         <v>43</v>
@@ -19111,7 +19111,7 @@
         <v>365</v>
       </c>
       <c r="G318" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H318" t="s">
         <v>43</v>
@@ -19164,7 +19164,7 @@
         <v>365</v>
       </c>
       <c r="G319" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H319" t="s">
         <v>43</v>
@@ -19217,7 +19217,7 @@
         <v>365</v>
       </c>
       <c r="G320" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H320" t="s">
         <v>43</v>
@@ -19270,7 +19270,7 @@
         <v>365</v>
       </c>
       <c r="G321" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H321" t="s">
         <v>43</v>
@@ -19323,7 +19323,7 @@
         <v>365</v>
       </c>
       <c r="G322" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H322" t="s">
         <v>43</v>
@@ -19376,7 +19376,7 @@
         <v>365</v>
       </c>
       <c r="G323" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H323" t="s">
         <v>43</v>
@@ -19429,7 +19429,7 @@
         <v>365</v>
       </c>
       <c r="G324" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H324" t="s">
         <v>43</v>
@@ -19482,7 +19482,7 @@
         <v>365</v>
       </c>
       <c r="G325" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H325" t="s">
         <v>43</v>
@@ -19535,7 +19535,7 @@
         <v>365</v>
       </c>
       <c r="G326" t="s">
-        <v>365</v>
+        <v>135</v>
       </c>
       <c r="H326" t="s">
         <v>43</v>
@@ -19588,7 +19588,7 @@
         <v>390</v>
       </c>
       <c r="G327" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H327" t="s">
         <v>43</v>
@@ -19615,15 +19615,15 @@
         <v>293</v>
       </c>
       <c r="P327" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="Q327" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B328" t="s">
         <v>18</v>
@@ -19641,7 +19641,7 @@
         <v>390</v>
       </c>
       <c r="G328" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H328" t="s">
         <v>43</v>
@@ -19668,15 +19668,15 @@
         <v>293</v>
       </c>
       <c r="P328" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="Q328" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B329" t="s">
         <v>18</v>
@@ -19694,7 +19694,7 @@
         <v>390</v>
       </c>
       <c r="G329" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H329" t="s">
         <v>43</v>
@@ -19721,15 +19721,15 @@
         <v>293</v>
       </c>
       <c r="P329" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="Q329" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B330" t="s">
         <v>18</v>
@@ -19744,10 +19744,10 @@
         <v>345</v>
       </c>
       <c r="F330" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G330" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="H330" t="s">
         <v>43</v>
@@ -19797,10 +19797,10 @@
         <v>346</v>
       </c>
       <c r="F331" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G331" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="H331" t="s">
         <v>43</v>
@@ -19850,10 +19850,10 @@
         <v>347</v>
       </c>
       <c r="F332" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G332" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="H332" t="s">
         <v>43</v>
@@ -19903,10 +19903,10 @@
         <v>348</v>
       </c>
       <c r="F333" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G333" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="H333" t="s">
         <v>43</v>
@@ -19956,10 +19956,10 @@
         <v>349</v>
       </c>
       <c r="F334" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G334" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="H334" t="s">
         <v>43</v>
@@ -20009,10 +20009,10 @@
         <v>350</v>
       </c>
       <c r="F335" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G335" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="H335" t="s">
         <v>43</v>
@@ -20062,10 +20062,10 @@
         <v>351</v>
       </c>
       <c r="F336" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G336" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="H336" t="s">
         <v>43</v>
@@ -20115,10 +20115,10 @@
         <v>352</v>
       </c>
       <c r="F337" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G337" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="H337" t="s">
         <v>43</v>
@@ -20168,10 +20168,10 @@
         <v>353</v>
       </c>
       <c r="F338" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G338" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="H338" t="s">
         <v>43</v>
@@ -20221,10 +20221,10 @@
         <v>354</v>
       </c>
       <c r="F339" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G339" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="H339" t="s">
         <v>43</v>
@@ -20277,7 +20277,7 @@
         <v>390</v>
       </c>
       <c r="G340" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H340" t="s">
         <v>43</v>
@@ -20304,10 +20304,10 @@
         <v>293</v>
       </c>
       <c r="P340" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="Q340" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="341">
@@ -20330,7 +20330,7 @@
         <v>390</v>
       </c>
       <c r="G341" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H341" t="s">
         <v>43</v>
@@ -20357,10 +20357,10 @@
         <v>293</v>
       </c>
       <c r="P341" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="Q341" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="342">
@@ -20383,7 +20383,7 @@
         <v>390</v>
       </c>
       <c r="G342" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H342" t="s">
         <v>43</v>
@@ -20410,10 +20410,10 @@
         <v>293</v>
       </c>
       <c r="P342" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="Q342" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="343">
@@ -20436,7 +20436,7 @@
         <v>390</v>
       </c>
       <c r="G343" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H343" t="s">
         <v>43</v>
@@ -20463,10 +20463,10 @@
         <v>293</v>
       </c>
       <c r="P343" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="Q343" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="344">
@@ -20489,7 +20489,7 @@
         <v>390</v>
       </c>
       <c r="G344" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H344" t="s">
         <v>43</v>
@@ -20516,10 +20516,10 @@
         <v>293</v>
       </c>
       <c r="P344" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="Q344" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="345">
@@ -20542,7 +20542,7 @@
         <v>390</v>
       </c>
       <c r="G345" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H345" t="s">
         <v>43</v>
@@ -20569,10 +20569,10 @@
         <v>293</v>
       </c>
       <c r="P345" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="Q345" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="346">
@@ -20595,7 +20595,7 @@
         <v>390</v>
       </c>
       <c r="G346" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H346" t="s">
         <v>43</v>
@@ -20622,10 +20622,10 @@
         <v>293</v>
       </c>
       <c r="P346" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="Q346" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="347">
@@ -20648,7 +20648,7 @@
         <v>390</v>
       </c>
       <c r="G347" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H347" t="s">
         <v>43</v>
@@ -20675,10 +20675,10 @@
         <v>293</v>
       </c>
       <c r="P347" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="Q347" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="348">
@@ -20701,7 +20701,7 @@
         <v>390</v>
       </c>
       <c r="G348" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H348" t="s">
         <v>43</v>
@@ -20728,10 +20728,10 @@
         <v>293</v>
       </c>
       <c r="P348" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="Q348" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="349">
@@ -20754,7 +20754,7 @@
         <v>390</v>
       </c>
       <c r="G349" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H349" t="s">
         <v>43</v>
@@ -20781,10 +20781,10 @@
         <v>293</v>
       </c>
       <c r="P349" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="Q349" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="350">
@@ -20804,10 +20804,10 @@
         <v>365</v>
       </c>
       <c r="F350" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G350" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="H350" t="s">
         <v>43</v>
@@ -20857,10 +20857,10 @@
         <v>366</v>
       </c>
       <c r="F351" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G351" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="H351" t="s">
         <v>43</v>
@@ -20910,10 +20910,10 @@
         <v>367</v>
       </c>
       <c r="F352" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G352" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="H352" t="s">
         <v>43</v>
@@ -20963,10 +20963,10 @@
         <v>368</v>
       </c>
       <c r="F353" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G353" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="H353" t="s">
         <v>43</v>
@@ -21016,10 +21016,10 @@
         <v>369</v>
       </c>
       <c r="F354" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G354" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="H354" t="s">
         <v>43</v>
@@ -21069,10 +21069,10 @@
         <v>370</v>
       </c>
       <c r="F355" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G355" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="H355" t="s">
         <v>43</v>
@@ -21122,10 +21122,10 @@
         <v>371</v>
       </c>
       <c r="F356" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G356" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="H356" t="s">
         <v>43</v>
@@ -21175,10 +21175,10 @@
         <v>372</v>
       </c>
       <c r="F357" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G357" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="H357" t="s">
         <v>43</v>
@@ -21231,7 +21231,7 @@
         <v>390</v>
       </c>
       <c r="G358" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H358" t="s">
         <v>43</v>
@@ -21258,10 +21258,10 @@
         <v>293</v>
       </c>
       <c r="P358" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="Q358" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="359">
@@ -21284,7 +21284,7 @@
         <v>390</v>
       </c>
       <c r="G359" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H359" t="s">
         <v>43</v>
@@ -21311,10 +21311,10 @@
         <v>293</v>
       </c>
       <c r="P359" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="Q359" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="360">
@@ -21337,7 +21337,7 @@
         <v>390</v>
       </c>
       <c r="G360" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H360" t="s">
         <v>43</v>
@@ -21364,10 +21364,10 @@
         <v>293</v>
       </c>
       <c r="P360" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="Q360" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="361">
@@ -21390,7 +21390,7 @@
         <v>390</v>
       </c>
       <c r="G361" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H361" t="s">
         <v>43</v>
@@ -21417,10 +21417,10 @@
         <v>293</v>
       </c>
       <c r="P361" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="Q361" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="362">
@@ -21440,10 +21440,10 @@
         <v>377</v>
       </c>
       <c r="F362" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G362" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="H362" t="s">
         <v>43</v>
@@ -21496,7 +21496,7 @@
         <v>101</v>
       </c>
       <c r="G363" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H363" t="s">
         <v>43</v>
@@ -21549,7 +21549,7 @@
         <v>202</v>
       </c>
       <c r="G364" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H364" t="s">
         <v>43</v>
@@ -21602,7 +21602,7 @@
         <v>202</v>
       </c>
       <c r="G365" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H365" t="s">
         <v>43</v>
@@ -21655,7 +21655,7 @@
         <v>101</v>
       </c>
       <c r="G366" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H366" t="s">
         <v>43</v>
@@ -21708,7 +21708,7 @@
         <v>101</v>
       </c>
       <c r="G367" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H367" t="s">
         <v>43</v>
@@ -21761,7 +21761,7 @@
         <v>101</v>
       </c>
       <c r="G368" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H368" t="s">
         <v>43</v>
@@ -21814,7 +21814,7 @@
         <v>101</v>
       </c>
       <c r="G369" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H369" t="s">
         <v>43</v>
@@ -21867,7 +21867,7 @@
         <v>101</v>
       </c>
       <c r="G370" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H370" t="s">
         <v>43</v>
@@ -21920,7 +21920,7 @@
         <v>202</v>
       </c>
       <c r="G371" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H371" t="s">
         <v>43</v>
@@ -21973,7 +21973,7 @@
         <v>202</v>
       </c>
       <c r="G372" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H372" t="s">
         <v>43</v>
@@ -22026,7 +22026,7 @@
         <v>202</v>
       </c>
       <c r="G373" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H373" t="s">
         <v>43</v>
@@ -22079,7 +22079,7 @@
         <v>101</v>
       </c>
       <c r="G374" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H374" t="s">
         <v>43</v>
@@ -22132,7 +22132,7 @@
         <v>101</v>
       </c>
       <c r="G375" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H375" t="s">
         <v>43</v>
@@ -22185,7 +22185,7 @@
         <v>149</v>
       </c>
       <c r="G376" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H376" t="s">
         <v>43</v>
@@ -22238,7 +22238,7 @@
         <v>149</v>
       </c>
       <c r="G377" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H377" t="s">
         <v>43</v>
@@ -22291,7 +22291,7 @@
         <v>149</v>
       </c>
       <c r="G378" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H378" t="s">
         <v>43</v>
@@ -22344,7 +22344,7 @@
         <v>149</v>
       </c>
       <c r="G379" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H379" t="s">
         <v>43</v>
@@ -22397,7 +22397,7 @@
         <v>135</v>
       </c>
       <c r="G380" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="H380" t="s">
         <v>43</v>
@@ -22450,7 +22450,7 @@
         <v>202</v>
       </c>
       <c r="G381" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H381" t="s">
         <v>43</v>
@@ -22503,7 +22503,7 @@
         <v>202</v>
       </c>
       <c r="G382" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H382" t="s">
         <v>43</v>
@@ -22556,7 +22556,7 @@
         <v>202</v>
       </c>
       <c r="G383" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H383" t="s">
         <v>43</v>
@@ -22609,7 +22609,7 @@
         <v>101</v>
       </c>
       <c r="G384" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H384" t="s">
         <v>43</v>
@@ -22662,7 +22662,7 @@
         <v>101</v>
       </c>
       <c r="G385" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H385" t="s">
         <v>43</v>
@@ -22715,7 +22715,7 @@
         <v>101</v>
       </c>
       <c r="G386" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H386" t="s">
         <v>43</v>
@@ -22768,7 +22768,7 @@
         <v>149</v>
       </c>
       <c r="G387" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H387" t="s">
         <v>43</v>
@@ -22821,7 +22821,7 @@
         <v>149</v>
       </c>
       <c r="G388" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H388" t="s">
         <v>43</v>
@@ -22874,7 +22874,7 @@
         <v>149</v>
       </c>
       <c r="G389" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H389" t="s">
         <v>43</v>
@@ -22927,7 +22927,7 @@
         <v>135</v>
       </c>
       <c r="G390" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="H390" t="s">
         <v>43</v>
@@ -22980,7 +22980,7 @@
         <v>135</v>
       </c>
       <c r="G391" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="H391" t="s">
         <v>43</v>
@@ -23033,7 +23033,7 @@
         <v>135</v>
       </c>
       <c r="G392" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="H392" t="s">
         <v>43</v>
@@ -23086,7 +23086,7 @@
         <v>202</v>
       </c>
       <c r="G393" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H393" t="s">
         <v>43</v>
@@ -23139,7 +23139,7 @@
         <v>202</v>
       </c>
       <c r="G394" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H394" t="s">
         <v>43</v>
@@ -23192,7 +23192,7 @@
         <v>202</v>
       </c>
       <c r="G395" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H395" t="s">
         <v>43</v>
@@ -23245,7 +23245,7 @@
         <v>202</v>
       </c>
       <c r="G396" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H396" t="s">
         <v>43</v>
@@ -23298,7 +23298,7 @@
         <v>202</v>
       </c>
       <c r="G397" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H397" t="s">
         <v>43</v>
@@ -23351,7 +23351,7 @@
         <v>101</v>
       </c>
       <c r="G398" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H398" t="s">
         <v>43</v>
@@ -23404,7 +23404,7 @@
         <v>101</v>
       </c>
       <c r="G399" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H399" t="s">
         <v>43</v>
@@ -23457,7 +23457,7 @@
         <v>101</v>
       </c>
       <c r="G400" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H400" t="s">
         <v>43</v>
@@ -23510,7 +23510,7 @@
         <v>149</v>
       </c>
       <c r="G401" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H401" t="s">
         <v>43</v>
@@ -23563,7 +23563,7 @@
         <v>149</v>
       </c>
       <c r="G402" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H402" t="s">
         <v>43</v>
@@ -23616,7 +23616,7 @@
         <v>135</v>
       </c>
       <c r="G403" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="H403" t="s">
         <v>43</v>
@@ -23669,7 +23669,7 @@
         <v>135</v>
       </c>
       <c r="G404" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="H404" t="s">
         <v>43</v>
@@ -23722,7 +23722,7 @@
         <v>202</v>
       </c>
       <c r="G405" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H405" t="s">
         <v>43</v>
@@ -23775,7 +23775,7 @@
         <v>202</v>
       </c>
       <c r="G406" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H406" t="s">
         <v>43</v>
@@ -23828,7 +23828,7 @@
         <v>202</v>
       </c>
       <c r="G407" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H407" t="s">
         <v>43</v>
@@ -23881,7 +23881,7 @@
         <v>101</v>
       </c>
       <c r="G408" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H408" t="s">
         <v>43</v>
@@ -23934,7 +23934,7 @@
         <v>101</v>
       </c>
       <c r="G409" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H409" t="s">
         <v>43</v>
@@ -23987,7 +23987,7 @@
         <v>101</v>
       </c>
       <c r="G410" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H410" t="s">
         <v>43</v>
@@ -24040,7 +24040,7 @@
         <v>101</v>
       </c>
       <c r="G411" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H411" t="s">
         <v>43</v>
@@ -24093,7 +24093,7 @@
         <v>101</v>
       </c>
       <c r="G412" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H412" t="s">
         <v>43</v>
@@ -24146,7 +24146,7 @@
         <v>149</v>
       </c>
       <c r="G413" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H413" t="s">
         <v>43</v>
@@ -24199,7 +24199,7 @@
         <v>149</v>
       </c>
       <c r="G414" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H414" t="s">
         <v>43</v>
@@ -24252,7 +24252,7 @@
         <v>149</v>
       </c>
       <c r="G415" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H415" t="s">
         <v>43</v>
@@ -24305,7 +24305,7 @@
         <v>135</v>
       </c>
       <c r="G416" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="H416" t="s">
         <v>43</v>
@@ -24358,7 +24358,7 @@
         <v>135</v>
       </c>
       <c r="G417" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="H417" t="s">
         <v>43</v>
@@ -24411,7 +24411,7 @@
         <v>135</v>
       </c>
       <c r="G418" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="H418" t="s">
         <v>43</v>
@@ -24464,7 +24464,7 @@
         <v>202</v>
       </c>
       <c r="G419" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H419" t="s">
         <v>43</v>
@@ -24517,7 +24517,7 @@
         <v>202</v>
       </c>
       <c r="G420" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H420" t="s">
         <v>43</v>
@@ -24570,7 +24570,7 @@
         <v>101</v>
       </c>
       <c r="G421" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H421" t="s">
         <v>43</v>
@@ -24623,7 +24623,7 @@
         <v>101</v>
       </c>
       <c r="G422" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H422" t="s">
         <v>43</v>
@@ -24676,7 +24676,7 @@
         <v>101</v>
       </c>
       <c r="G423" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H423" t="s">
         <v>43</v>
@@ -24729,7 +24729,7 @@
         <v>101</v>
       </c>
       <c r="G424" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="H424" t="s">
         <v>43</v>
@@ -24782,7 +24782,7 @@
         <v>149</v>
       </c>
       <c r="G425" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H425" t="s">
         <v>43</v>
@@ -24835,7 +24835,7 @@
         <v>149</v>
       </c>
       <c r="G426" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H426" t="s">
         <v>43</v>
@@ -24888,7 +24888,7 @@
         <v>149</v>
       </c>
       <c r="G427" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H427" t="s">
         <v>43</v>
@@ -24941,7 +24941,7 @@
         <v>149</v>
       </c>
       <c r="G428" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H428" t="s">
         <v>43</v>
@@ -24994,7 +24994,7 @@
         <v>135</v>
       </c>
       <c r="G429" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="H429" t="s">
         <v>43</v>
@@ -25047,7 +25047,7 @@
         <v>135</v>
       </c>
       <c r="G430" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="H430" t="s">
         <v>43</v>
@@ -25100,7 +25100,7 @@
         <v>202</v>
       </c>
       <c r="G431" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H431" t="s">
         <v>43</v>
@@ -25153,7 +25153,7 @@
         <v>202</v>
       </c>
       <c r="G432" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H432" t="s">
         <v>43</v>
@@ -25206,7 +25206,7 @@
         <v>202</v>
       </c>
       <c r="G433" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H433" t="s">
         <v>43</v>
@@ -25259,7 +25259,7 @@
         <v>202</v>
       </c>
       <c r="G434" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="H434" t="s">
         <v>43</v>
@@ -25312,7 +25312,7 @@
         <v>149</v>
       </c>
       <c r="G435" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H435" t="s">
         <v>43</v>
@@ -25365,7 +25365,7 @@
         <v>149</v>
       </c>
       <c r="G436" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H436" t="s">
         <v>43</v>
@@ -25418,7 +25418,7 @@
         <v>149</v>
       </c>
       <c r="G437" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H437" t="s">
         <v>43</v>
@@ -25471,7 +25471,7 @@
         <v>149</v>
       </c>
       <c r="G438" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H438" t="s">
         <v>43</v>
@@ -25524,7 +25524,7 @@
         <v>149</v>
       </c>
       <c r="G439" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H439" t="s">
         <v>43</v>
@@ -25577,7 +25577,7 @@
         <v>149</v>
       </c>
       <c r="G440" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H440" t="s">
         <v>43</v>
@@ -25630,7 +25630,7 @@
         <v>149</v>
       </c>
       <c r="G441" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H441" t="s">
         <v>43</v>
@@ -25683,7 +25683,7 @@
         <v>135</v>
       </c>
       <c r="G442" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="H442" t="s">
         <v>43</v>
@@ -25736,7 +25736,7 @@
         <v>135</v>
       </c>
       <c r="G443" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="H443" t="s">
         <v>43</v>
@@ -25789,7 +25789,7 @@
         <v>135</v>
       </c>
       <c r="G444" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="H444" t="s">
         <v>43</v>
@@ -25842,7 +25842,7 @@
         <v>149</v>
       </c>
       <c r="G445" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="H445" t="s">
         <v>43</v>
@@ -25895,7 +25895,7 @@
         <v>135</v>
       </c>
       <c r="G446" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="H446" t="s">
         <v>43</v>
@@ -25948,7 +25948,7 @@
         <v>135</v>
       </c>
       <c r="G447" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="H447" t="s">
         <v>43</v>
@@ -26001,7 +26001,7 @@
         <v>135</v>
       </c>
       <c r="G448" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="H448" t="s">
         <v>43</v>
@@ -26054,7 +26054,7 @@
         <v>135</v>
       </c>
       <c r="G449" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="H449" t="s">
         <v>43</v>
@@ -26107,7 +26107,7 @@
         <v>135</v>
       </c>
       <c r="G450" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="H450" t="s">
         <v>43</v>
@@ -26160,7 +26160,7 @@
         <v>135</v>
       </c>
       <c r="G451" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="H451" t="s">
         <v>43</v>
@@ -28224,10 +28224,10 @@
         <v>505</v>
       </c>
       <c r="F490" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G490" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="H490" t="s">
         <v>22</v>
@@ -28277,10 +28277,10 @@
         <v>506</v>
       </c>
       <c r="F491" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G491" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="H491" t="s">
         <v>22</v>
@@ -28330,10 +28330,10 @@
         <v>507</v>
       </c>
       <c r="F492" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G492" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="H492" t="s">
         <v>22</v>
@@ -28383,10 +28383,10 @@
         <v>508</v>
       </c>
       <c r="F493" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G493" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="H493" t="s">
         <v>22</v>
@@ -28436,10 +28436,10 @@
         <v>509</v>
       </c>
       <c r="F494" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G494" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="H494" t="s">
         <v>22</v>
@@ -28489,10 +28489,10 @@
         <v>510</v>
       </c>
       <c r="F495" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G495" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="H495" t="s">
         <v>22</v>
@@ -28542,10 +28542,10 @@
         <v>511</v>
       </c>
       <c r="F496" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G496" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="H496" t="s">
         <v>22</v>

</xml_diff>